<commit_message>
Update BLAPE and RPEpUACE based on 2020 GHG Inventory data
</commit_message>
<xml_diff>
--- a/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
+++ b/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\land\RPEpUACE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\RPEpUACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0C39C8-7140-4E9A-800C-6D86145E4794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="383" yWindow="83" windowWidth="19140" windowHeight="9263"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="RPEpUACE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>RPEpUACE Rebound Pollutant Emissions per Unit Avoided CO2 Emissions</t>
   </si>
@@ -59,61 +72,157 @@
     <t>Unit: kt</t>
   </si>
   <si>
+    <t>VOC</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>NOx</t>
+  </si>
+  <si>
+    <t>PM10</t>
+  </si>
+  <si>
+    <t>PM25</t>
+  </si>
+  <si>
+    <t>SOx</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>F gases</t>
+  </si>
+  <si>
+    <t>Rebound Emis Factor (dimensionless)</t>
+  </si>
+  <si>
+    <t>US EPA</t>
+  </si>
+  <si>
+    <t>Table 6-3</t>
+  </si>
+  <si>
+    <t>Table 6-3:  Emissions and Removals from Land Use, Land-Use Change, and Forestry by Gas (kt)</t>
+  </si>
+  <si>
+    <t>Gas/Land-Use Category</t>
+  </si>
+  <si>
+    <t>Carbon Stock Change (CO2)a</t>
+  </si>
+  <si>
+    <t>Forest Land Remaining Forest Land</t>
+  </si>
+  <si>
+    <t>Land Converted to Forest Land</t>
+  </si>
+  <si>
+    <t>Cropland Remaining Cropland</t>
+  </si>
+  <si>
+    <t>Land Converted to Cropland</t>
+  </si>
+  <si>
+    <t>Grassland Remaining Grassland</t>
+  </si>
+  <si>
+    <t>Land Converted to Grassland</t>
+  </si>
+  <si>
+    <t>Wetlands Remaining Wetlands</t>
+  </si>
+  <si>
+    <t>Land Converted to Wetlands</t>
+  </si>
+  <si>
+    <t>Settlements Remaining Settlements</t>
+  </si>
+  <si>
+    <t>Land Converted to Settlements</t>
+  </si>
+  <si>
+    <t>Forest Land Remaining Forest Land: Forest Firesb</t>
+  </si>
+  <si>
+    <t>Forest Land Remaining Forest Land: Drained Organic Soilsd</t>
+  </si>
+  <si>
+    <t>Grassland Remaining Grassland: Grassland Firesc</t>
+  </si>
+  <si>
+    <t>Wetlands Remaining Wetlands: Flooded Land Remaining Flooded Land</t>
+  </si>
+  <si>
+    <t>Wetlands Remaining Wetlands: Coastal Wetlands Remaining Coastal Wetlands</t>
+  </si>
+  <si>
+    <t>Wetlands Remaining Wetlands: Peatlands Remaining Peatlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ </t>
+  </si>
+  <si>
+    <t>Land Converted to Wetlands: Land Converted to Flooded Lands</t>
+  </si>
+  <si>
+    <t>Land Converted to Wetlands: Land Converted to Coastal Wetlands</t>
+  </si>
+  <si>
+    <t>Forest Land Remaining Forest Land: Forest Soilsf</t>
+  </si>
+  <si>
+    <t>Settlements Remaining Settlements: Settlement Soilse</t>
+  </si>
+  <si>
+    <t>+ Absolute value does not exceed 0.5 kt.</t>
+  </si>
+  <si>
+    <t>a LULUCF Carbon Stock Change is the net C stock change from the following categories: Forest Land Remaining Forest Land, Land Converted to Forest Land, Cropland Remaining Cropland, Land Converted to Cropland, Grassland Remaining Grassland, Land Converted to Grassland, Wetlands Remaining Wetlands, Land Converted to Wetlands, Settlements Remaining Settlements, and Land Converted to Settlements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b Estimates include CH4 and N2O emissions from fires on both Forest Land Remaining Forest Land and Land Converted to Forest Land. </t>
+  </si>
+  <si>
+    <t>c Estimates include CH4 and N2O emissions from drained organic soils on both Forest Land Remaining Forest Land and Land Converted to Forest Land.</t>
+  </si>
+  <si>
+    <t>d Estimates include CH4 and N2O emissions from fires on both Grassland Remaining Grassland and Land Converted to Grassland.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e Estimates include N2O emissions from N fertilizer additions on both Forest Land Remaining Forest Land and Land Converted to Forest Land. </t>
+  </si>
+  <si>
+    <t>f Estimates include N2O emissions from N fertilizer additions on both Settlements Remaining Settlements and Land Converted to Settlements.</t>
+  </si>
+  <si>
+    <t>Notes: Totals may not sum due to independent rounding. Parentheses indicate net sequestration.</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/ghgemissions/inventory-us-greenhouse-gas-emissions-and-sinks-1990-2020</t>
+  </si>
+  <si>
+    <t>Table 6-3:</t>
+  </si>
+  <si>
+    <t>Inventory of US Greenhouse Gas Emissions Emissions and Sinks: 1990-2020</t>
+  </si>
+  <si>
     <t>CH4/CO2 Ratio</t>
   </si>
   <si>
     <t>N2O/CO2 Ratio</t>
-  </si>
-  <si>
-    <t>VOC</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>NOx</t>
-  </si>
-  <si>
-    <t>PM10</t>
-  </si>
-  <si>
-    <t>PM25</t>
-  </si>
-  <si>
-    <t>SOx</t>
-  </si>
-  <si>
-    <t>BC</t>
-  </si>
-  <si>
-    <t>OC</t>
-  </si>
-  <si>
-    <t>F gases</t>
-  </si>
-  <si>
-    <t>Rebound Emis Factor (dimensionless)</t>
-  </si>
-  <si>
-    <t>Excerpt from Table 6-2:</t>
-  </si>
-  <si>
-    <t>US EPA</t>
-  </si>
-  <si>
-    <t>Draft Inventory of US Greenhouse Gas Emissions Emissions and Sinks</t>
-  </si>
-  <si>
-    <t>https://www.epa.gov/sites/production/files/2021-02/documents/us-ghg-inventory-2021-main-text.pdf</t>
-  </si>
-  <si>
-    <t>Table 6-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -168,6 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -262,6 +372,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -297,6 +424,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -472,236 +616,781 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.19921875" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B3">
-        <v>2015</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
         <v>2016</v>
       </c>
-      <c r="D3">
+      <c r="C4">
         <v>2017</v>
       </c>
-      <c r="E3">
+      <c r="D4">
         <v>2018</v>
       </c>
-      <c r="F3">
+      <c r="E4">
         <v>2019</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="F4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-862045</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-826667</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-809026</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-760820</v>
+      </c>
+      <c r="F5" s="5">
+        <v>-812176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-725571</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-688301</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-677101</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-634824</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-668057</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-99454</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-99523</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-99518</v>
+      </c>
+      <c r="E7" s="5">
+        <v>-99520</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-99521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-22731</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-22293</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-16597</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-14544</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-23335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5">
+        <v>54107</v>
+      </c>
+      <c r="C9" s="5">
+        <v>54273</v>
+      </c>
+      <c r="D9" s="5">
+        <v>53975</v>
+      </c>
+      <c r="E9" s="5">
+        <v>53935</v>
+      </c>
+      <c r="F9" s="5">
+        <v>54380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5">
+        <v>7958</v>
+      </c>
+      <c r="C10" s="5">
+        <v>9308</v>
+      </c>
+      <c r="D10" s="5">
+        <v>9670</v>
+      </c>
+      <c r="E10" s="5">
+        <v>12425</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-22553</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-22693</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-22397</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-21485</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-24101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5">
+        <v>-8046</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-7954</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-7994</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-8034</v>
+      </c>
+      <c r="F12" s="5">
+        <v>-8084</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>254</v>
+      </c>
+      <c r="C13">
+        <v>258</v>
+      </c>
+      <c r="D13">
+        <v>265</v>
+      </c>
+      <c r="E13">
+        <v>271</v>
+      </c>
+      <c r="F13">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-123794</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-127679</v>
+      </c>
+      <c r="D14" s="5">
+        <v>-127299</v>
+      </c>
+      <c r="E14" s="5">
+        <v>-126977</v>
+      </c>
+      <c r="F14" s="5">
+        <v>-126128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5">
+        <v>77784</v>
+      </c>
+      <c r="C15" s="5">
+        <v>77938</v>
+      </c>
+      <c r="D15" s="5">
+        <v>77970</v>
+      </c>
+      <c r="E15" s="5">
+        <v>77932</v>
+      </c>
+      <c r="F15" s="5">
+        <v>77895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1131</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1359</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1226</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1022</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>154</v>
+      </c>
+      <c r="C17">
+        <v>381</v>
+      </c>
+      <c r="D17">
+        <v>249</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>796.7</v>
+      </c>
+      <c r="C20">
+        <v>796.8</v>
+      </c>
+      <c r="D20">
+        <v>796.9</v>
+      </c>
+      <c r="E20">
+        <v>796.9</v>
+      </c>
+      <c r="F20">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>153</v>
+      </c>
+      <c r="C21">
+        <v>153</v>
+      </c>
+      <c r="D21">
+        <v>153</v>
+      </c>
+      <c r="E21">
+        <v>153</v>
+      </c>
+      <c r="F21">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>-791695</v>
-      </c>
-      <c r="C4">
-        <v>-855998</v>
-      </c>
-      <c r="D4">
-        <v>-792046</v>
-      </c>
-      <c r="E4">
-        <v>-824885</v>
-      </c>
-      <c r="F4">
-        <v>-812695</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>663</v>
-      </c>
-      <c r="C5">
-        <v>308</v>
-      </c>
-      <c r="D5">
-        <v>614</v>
-      </c>
-      <c r="E5">
-        <v>552</v>
-      </c>
-      <c r="F5">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>39</v>
+      </c>
+      <c r="D25">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>36</v>
-      </c>
-      <c r="E6">
-        <v>32</v>
-      </c>
-      <c r="F6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
-        <f>B5/B4</f>
-        <v>-8.3744371254081433E-4</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:F8" si="0">C5/C4</f>
-        <v>-3.5981392479888971E-4</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="3">
+        <f>B16/B5</f>
+        <v>-1.3119964735019633E-3</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" ref="C43:F43" si="0">C16/C5</f>
+        <v>-1.6439509500197783E-3</v>
+      </c>
+      <c r="D43" s="3">
         <f t="shared" si="0"/>
-        <v>-7.7520750057446164E-4</v>
-      </c>
-      <c r="E8" s="3">
+        <v>-1.5154024716140149E-3</v>
+      </c>
+      <c r="E43" s="3">
         <f t="shared" si="0"/>
-        <v>-6.6918418931123734E-4</v>
-      </c>
-      <c r="F8" s="3">
+        <v>-1.3432875055860781E-3</v>
+      </c>
+      <c r="F43" s="3">
         <f t="shared" si="0"/>
-        <v>-6.7922160220008736E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
-        <f>B6/B4</f>
-        <v>-4.7998282166743506E-5</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" ref="C9:F9" si="1">C6/C4</f>
-        <v>-2.1028086514220829E-5</v>
-      </c>
-      <c r="D9" s="3">
+        <v>-1.8739780540178485E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="3">
+        <f>B25/B5</f>
+        <v>-2.7840773973516463E-5</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" ref="C44:F44" si="1">C25/C5</f>
+        <v>-4.7177400331693413E-5</v>
+      </c>
+      <c r="D44" s="3">
         <f t="shared" si="1"/>
-        <v>-4.5451905571141073E-5</v>
-      </c>
-      <c r="E9" s="3">
+        <v>-3.8317680766749151E-5</v>
+      </c>
+      <c r="E44" s="3">
         <f t="shared" si="1"/>
-        <v>-3.8793286336883321E-5</v>
-      </c>
-      <c r="F9" s="3">
+        <v>-2.1029941379038406E-5</v>
+      </c>
+      <c r="F44" s="3">
         <f t="shared" si="1"/>
-        <v>-3.9375165344932599E-5</v>
+        <v>-6.2794271192450897E-5</v>
       </c>
     </row>
   </sheetData>
@@ -710,27 +1399,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -738,91 +1427,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <f>-AVERAGE(Data!B8:F8)</f>
-        <v>6.6417418588509813E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <f>-AVERAGE(Data!B43:F43)</f>
+        <v>1.5377230909479366E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <f>-AVERAGE(Data!B9:F9)</f>
-        <v>3.8529345186784264E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <f>-AVERAGE(Data!B44:F44)</f>
+        <v>3.9432013528689668E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>